<commit_message>
Added results for Kochia 8 bands
</commit_message>
<xml_diff>
--- a/Kochia/results/Summary.xlsx
+++ b/Kochia/results/Summary.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\w63x712\Documents\Machine_Learning\HSI_selection2\Kochia\results\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{59B18522-DF4C-407E-A6FD-E98CC0398B8A}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6FAEE81E-BB6C-4066-ADB2-DCEED20ACDB6}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="28680" yWindow="-120" windowWidth="20640" windowHeight="11160" tabRatio="662" firstSheet="12" activeTab="16" xr2:uid="{D4E1857A-7969-4B6E-A5E0-8AB94818FDA4}"/>
   </bookViews>
@@ -50,7 +50,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2018" uniqueCount="1449">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2350" uniqueCount="1721">
   <si>
     <t>150 bands</t>
   </si>
@@ -4397,6 +4397,822 @@
   </si>
   <si>
     <t>87.872% (+/- 1.534%)</t>
+  </si>
+  <si>
+    <t>94.075% (+/- 0.602%)</t>
+  </si>
+  <si>
+    <t>94.667% (+/- 0.568%)</t>
+  </si>
+  <si>
+    <t>94.544% (+/- 0.535%)</t>
+  </si>
+  <si>
+    <t>94.597% (+/- 0.537%)</t>
+  </si>
+  <si>
+    <t>91.590% (+/- 1.250%)</t>
+  </si>
+  <si>
+    <t>92.519% (+/- 1.053%)</t>
+  </si>
+  <si>
+    <t>91.875% (+/- 1.240%)</t>
+  </si>
+  <si>
+    <t>92.167% (+/- 1.155%)</t>
+  </si>
+  <si>
+    <t>92.815% (+/- 0.789%)</t>
+  </si>
+  <si>
+    <t>93.407% (+/- 0.694%)</t>
+  </si>
+  <si>
+    <t>92.919% (+/- 0.912%)</t>
+  </si>
+  <si>
+    <t>93.145% (+/- 0.801%)</t>
+  </si>
+  <si>
+    <t>93.046% (+/- 0.898%)</t>
+  </si>
+  <si>
+    <t>93.855% (+/- 0.804%)</t>
+  </si>
+  <si>
+    <t>93.425% (+/- 0.839%)</t>
+  </si>
+  <si>
+    <t>93.616% (+/- 0.829%)</t>
+  </si>
+  <si>
+    <t>92.888% (+/- 0.710%)</t>
+  </si>
+  <si>
+    <t>93.451% (+/- 0.644%)</t>
+  </si>
+  <si>
+    <t>93.210% (+/- 0.674%)</t>
+  </si>
+  <si>
+    <t>93.320% (+/- 0.648%)</t>
+  </si>
+  <si>
+    <t>92.878% (+/- 0.548%)</t>
+  </si>
+  <si>
+    <t>93.628% (+/- 0.547%)</t>
+  </si>
+  <si>
+    <t>93.095% (+/- 0.460%)</t>
+  </si>
+  <si>
+    <t>93.340% (+/- 0.499%)</t>
+  </si>
+  <si>
+    <t>93.116% (+/- 0.322%)</t>
+  </si>
+  <si>
+    <t>93.690% (+/- 0.277%)</t>
+  </si>
+  <si>
+    <t>93.126% (+/- 0.457%)</t>
+  </si>
+  <si>
+    <t>93.388% (+/- 0.343%)</t>
+  </si>
+  <si>
+    <t>91.013% (+/- 1.370%)</t>
+  </si>
+  <si>
+    <t>91.974% (+/- 1.282%)</t>
+  </si>
+  <si>
+    <t>91.543% (+/- 1.351%)</t>
+  </si>
+  <si>
+    <t>91.745% (+/- 1.312%)</t>
+  </si>
+  <si>
+    <t>92.308% (+/- 0.832%)</t>
+  </si>
+  <si>
+    <t>92.997% (+/- 0.814%)</t>
+  </si>
+  <si>
+    <t>92.732% (+/- 0.890%)</t>
+  </si>
+  <si>
+    <t>92.855% (+/- 0.834%)</t>
+  </si>
+  <si>
+    <t>90.526% (+/- 1.648%)</t>
+  </si>
+  <si>
+    <t>91.701% (+/- 1.370%)</t>
+  </si>
+  <si>
+    <t>91.008% (+/- 1.722%)</t>
+  </si>
+  <si>
+    <t>91.321% (+/- 1.566%)</t>
+  </si>
+  <si>
+    <t>91.919% (+/- 0.813%)</t>
+  </si>
+  <si>
+    <t>92.689% (+/- 0.713%)</t>
+  </si>
+  <si>
+    <t>92.210% (+/- 0.868%)</t>
+  </si>
+  <si>
+    <t>92.427% (+/- 0.793%)</t>
+  </si>
+  <si>
+    <t>8 bands: 100% dataset</t>
+  </si>
+  <si>
+    <t>8 bands: 75% dataset</t>
+  </si>
+  <si>
+    <t>[2, 5, 18, 31, 54, 65, 68, 74]</t>
+  </si>
+  <si>
+    <t>91.499% (+/- 0.876%)</t>
+  </si>
+  <si>
+    <t>92.197% (+/- 0.822%)</t>
+  </si>
+  <si>
+    <t>92.077% (+/- 0.819%)</t>
+  </si>
+  <si>
+    <t>92.121% (+/- 0.805%)</t>
+  </si>
+  <si>
+    <t>93.200% (+/- 0.550%)</t>
+  </si>
+  <si>
+    <t>93.723% (+/- 0.508%)</t>
+  </si>
+  <si>
+    <t>92.913% (+/- 0.599%)</t>
+  </si>
+  <si>
+    <t>93.369% (+/- 0.706%)</t>
+  </si>
+  <si>
+    <t>93.162% (+/- 0.678%)</t>
+  </si>
+  <si>
+    <t>93.249% (+/- 0.658%)</t>
+  </si>
+  <si>
+    <t>[1, 18, 43, 67, 74, 78, 81, 143]</t>
+  </si>
+  <si>
+    <t>93.360% (+/- 0.675%)</t>
+  </si>
+  <si>
+    <t>93.869% (+/- 0.608%)</t>
+  </si>
+  <si>
+    <t>93.712% (+/- 0.693%)</t>
+  </si>
+  <si>
+    <t>93.775% (+/- 0.647%)</t>
+  </si>
+  <si>
+    <t>93.238% (+/- 0.865%)</t>
+  </si>
+  <si>
+    <t>93.849% (+/- 0.721%)</t>
+  </si>
+  <si>
+    <t>93.715% (+/- 0.954%)</t>
+  </si>
+  <si>
+    <t>93.772% (+/- 0.817%)</t>
+  </si>
+  <si>
+    <t>[0, 4, 18, 31, 43, 63, 68, 74]</t>
+  </si>
+  <si>
+    <t>93.284% (+/- 0.618%)</t>
+  </si>
+  <si>
+    <t>93.933% (+/- 0.519%)</t>
+  </si>
+  <si>
+    <t>93.773% (+/- 0.556%)</t>
+  </si>
+  <si>
+    <t>93.842% (+/- 0.530%)</t>
+  </si>
+  <si>
+    <t>93.474% (+/- 0.587%)</t>
+  </si>
+  <si>
+    <t>94.151% (+/- 0.442%)</t>
+  </si>
+  <si>
+    <t>93.849% (+/- 0.597%)</t>
+  </si>
+  <si>
+    <t>93.983% (+/- 0.510%)</t>
+  </si>
+  <si>
+    <t>92.035% (+/- 0.598%)</t>
+  </si>
+  <si>
+    <t>92.650% (+/- 0.450%)</t>
+  </si>
+  <si>
+    <t>92.378% (+/- 0.589%)</t>
+  </si>
+  <si>
+    <t>92.492% (+/- 0.486%)</t>
+  </si>
+  <si>
+    <t>93.567% (+/- 0.634%)</t>
+  </si>
+  <si>
+    <t>93.636% (+/- 0.567%)</t>
+  </si>
+  <si>
+    <t>8 bands: 50% dataset</t>
+  </si>
+  <si>
+    <t>90.437% (+/- 0.718%)</t>
+  </si>
+  <si>
+    <t>91.278% (+/- 0.624%)</t>
+  </si>
+  <si>
+    <t>91.034% (+/- 0.706%)</t>
+  </si>
+  <si>
+    <t>91.116% (+/- 0.655%)</t>
+  </si>
+  <si>
+    <t>90.437% (+/- 1.010%)</t>
+  </si>
+  <si>
+    <t>91.249% (+/- 0.903%)</t>
+  </si>
+  <si>
+    <t>90.958% (+/- 1.042%)</t>
+  </si>
+  <si>
+    <t>91.062% (+/- 0.957%)</t>
+  </si>
+  <si>
+    <t>90.418% (+/- 0.956%)</t>
+  </si>
+  <si>
+    <t>91.206% (+/- 0.871%)</t>
+  </si>
+  <si>
+    <t>90.716% (+/- 0.997%)</t>
+  </si>
+  <si>
+    <t>90.934% (+/- 0.920%)</t>
+  </si>
+  <si>
+    <t>90.621% (+/- 0.828%)</t>
+  </si>
+  <si>
+    <t>91.402% (+/- 0.736%)</t>
+  </si>
+  <si>
+    <t>91.055% (+/- 0.738%)</t>
+  </si>
+  <si>
+    <t>91.188% (+/- 0.736%)</t>
+  </si>
+  <si>
+    <t>91.355% (+/- 0.514%)</t>
+  </si>
+  <si>
+    <t>92.180% (+/- 0.475%)</t>
+  </si>
+  <si>
+    <t>91.973% (+/- 0.606%)</t>
+  </si>
+  <si>
+    <t>92.052% (+/- 0.518%)</t>
+  </si>
+  <si>
+    <t>91.279% (+/- 1.037%)</t>
+  </si>
+  <si>
+    <t>91.955% (+/- 0.886%)</t>
+  </si>
+  <si>
+    <t>91.962% (+/- 1.016%)</t>
+  </si>
+  <si>
+    <t>91.932% (+/- 0.939%)</t>
+  </si>
+  <si>
+    <t>90.918% (+/- 1.032%)</t>
+  </si>
+  <si>
+    <t>91.899% (+/- 0.854%)</t>
+  </si>
+  <si>
+    <t>91.416% (+/- 1.068%)</t>
+  </si>
+  <si>
+    <t>91.616% (+/- 0.961%)</t>
+  </si>
+  <si>
+    <t>89.158% (+/- 1.139%)</t>
+  </si>
+  <si>
+    <t>90.061% (+/- 0.955%)</t>
+  </si>
+  <si>
+    <t>89.576% (+/- 1.150%)</t>
+  </si>
+  <si>
+    <t>89.753% (+/- 1.041%)</t>
+  </si>
+  <si>
+    <t>93.200% (+/- 0.612%)</t>
+  </si>
+  <si>
+    <t>93.813% (+/- 0.394%)</t>
+  </si>
+  <si>
+    <t>93.480% (+/- 0.789%)</t>
+  </si>
+  <si>
+    <t>93.627% (+/- 0.599%)</t>
+  </si>
+  <si>
+    <t>90.101% (+/- 0.742%)</t>
+  </si>
+  <si>
+    <t>90.912% (+/- 0.621%)</t>
+  </si>
+  <si>
+    <t>90.875% (+/- 0.837%)</t>
+  </si>
+  <si>
+    <t>90.874% (+/- 0.687%)</t>
+  </si>
+  <si>
+    <t>90.426% (+/- 1.760%)</t>
+  </si>
+  <si>
+    <t>91.342% (+/- 1.637%)</t>
+  </si>
+  <si>
+    <t>90.732% (+/- 1.690%)</t>
+  </si>
+  <si>
+    <t>91.006% (+/- 1.650%)</t>
+  </si>
+  <si>
+    <t>91.169% (+/- 0.677%)</t>
+  </si>
+  <si>
+    <t>91.608% (+/- 0.755%)</t>
+  </si>
+  <si>
+    <t>91.404% (+/- 0.762%)</t>
+  </si>
+  <si>
+    <t>91.488% (+/- 0.689%)</t>
+  </si>
+  <si>
+    <t>91.477% (+/- 0.666%)</t>
+  </si>
+  <si>
+    <t>92.277% (+/- 0.724%)</t>
+  </si>
+  <si>
+    <t>91.949% (+/- 0.647%)</t>
+  </si>
+  <si>
+    <t>92.095% (+/- 0.638%)</t>
+  </si>
+  <si>
+    <t>8 bands: 25% dataset</t>
+  </si>
+  <si>
+    <t>85.684% (+/- 1.538%)</t>
+  </si>
+  <si>
+    <t>87.017% (+/- 1.297%)</t>
+  </si>
+  <si>
+    <t>86.037% (+/- 1.565%)</t>
+  </si>
+  <si>
+    <t>86.428% (+/- 1.473%)</t>
+  </si>
+  <si>
+    <t>85.975% (+/- 1.168%)</t>
+  </si>
+  <si>
+    <t>87.128% (+/- 1.204%)</t>
+  </si>
+  <si>
+    <t>86.364% (+/- 1.254%)</t>
+  </si>
+  <si>
+    <t>86.650% (+/- 1.239%)</t>
+  </si>
+  <si>
+    <t>85.975% (+/- 1.042%)</t>
+  </si>
+  <si>
+    <t>87.047% (+/- 1.211%)</t>
+  </si>
+  <si>
+    <t>85.936% (+/- 1.074%)</t>
+  </si>
+  <si>
+    <t>86.368% (+/- 1.100%)</t>
+  </si>
+  <si>
+    <t>86.532% (+/- 0.948%)</t>
+  </si>
+  <si>
+    <t>87.713% (+/- 1.014%)</t>
+  </si>
+  <si>
+    <t>86.641% (+/- 1.112%)</t>
+  </si>
+  <si>
+    <t>87.046% (+/- 1.038%)</t>
+  </si>
+  <si>
+    <t>86.316% (+/- 1.137%)</t>
+  </si>
+  <si>
+    <t>87.532% (+/- 1.147%)</t>
+  </si>
+  <si>
+    <t>86.757% (+/- 1.255%)</t>
+  </si>
+  <si>
+    <t>87.048% (+/- 1.202%)</t>
+  </si>
+  <si>
+    <t>[0, 4, 18, 43, 74, 79, 140, 146]</t>
+  </si>
+  <si>
+    <t>89.455% (+/- 0.930%)</t>
+  </si>
+  <si>
+    <t>90.564% (+/- 0.843%)</t>
+  </si>
+  <si>
+    <t>89.952% (+/- 0.780%)</t>
+  </si>
+  <si>
+    <t>90.238% (+/- 0.771%)</t>
+  </si>
+  <si>
+    <t>90.266% (+/- 0.622%)</t>
+  </si>
+  <si>
+    <t>91.004% (+/- 0.598%)</t>
+  </si>
+  <si>
+    <t>90.497% (+/- 0.665%)</t>
+  </si>
+  <si>
+    <t>90.731% (+/- 0.621%)</t>
+  </si>
+  <si>
+    <t>88.936% (+/- 0.950%)</t>
+  </si>
+  <si>
+    <t>90.065% (+/- 0.897%)</t>
+  </si>
+  <si>
+    <t>89.556% (+/- 1.015%)</t>
+  </si>
+  <si>
+    <t>89.793% (+/- 0.933%)</t>
+  </si>
+  <si>
+    <t>90.481% (+/- 0.761%)</t>
+  </si>
+  <si>
+    <t>91.453% (+/- 0.690%)</t>
+  </si>
+  <si>
+    <t>90.920% (+/- 0.861%)</t>
+  </si>
+  <si>
+    <t>91.166% (+/- 0.759%)</t>
+  </si>
+  <si>
+    <t>91.579% (+/- 0.568%)</t>
+  </si>
+  <si>
+    <t>92.384% (+/- 0.578%)</t>
+  </si>
+  <si>
+    <t>91.882% (+/- 0.650%)</t>
+  </si>
+  <si>
+    <t>92.109% (+/- 0.579%)</t>
+  </si>
+  <si>
+    <t>91.612% (+/- 0.658%)</t>
+  </si>
+  <si>
+    <t>92.268% (+/- 0.598%)</t>
+  </si>
+  <si>
+    <t>91.734% (+/- 0.770%)</t>
+  </si>
+  <si>
+    <t>91.979% (+/- 0.657%)</t>
+  </si>
+  <si>
+    <t>88.676% (+/- 1.125%)</t>
+  </si>
+  <si>
+    <t>89.761% (+/- 1.083%)</t>
+  </si>
+  <si>
+    <t>88.850% (+/- 1.177%)</t>
+  </si>
+  <si>
+    <t>89.245% (+/- 1.105%)</t>
+  </si>
+  <si>
+    <t>88.942% (+/- 0.872%)</t>
+  </si>
+  <si>
+    <t>89.769% (+/- 0.792%)</t>
+  </si>
+  <si>
+    <t>89.031% (+/- 0.888%)</t>
+  </si>
+  <si>
+    <t>89.348% (+/- 0.810%)</t>
+  </si>
+  <si>
+    <t>84.722% (+/- 0.942%)</t>
+  </si>
+  <si>
+    <t>86.280% (+/- 1.183%)</t>
+  </si>
+  <si>
+    <t>84.612% (+/- 1.056%)</t>
+  </si>
+  <si>
+    <t>85.251% (+/- 1.015%)</t>
+  </si>
+  <si>
+    <t>84.823% (+/- 1.097%)</t>
+  </si>
+  <si>
+    <t>85.914% (+/- 1.079%)</t>
+  </si>
+  <si>
+    <t>84.604% (+/- 1.269%)</t>
+  </si>
+  <si>
+    <t>85.134% (+/- 1.145%)</t>
+  </si>
+  <si>
+    <t>86.897% (+/- 1.386%)</t>
+  </si>
+  <si>
+    <t>88.406% (+/- 1.081%)</t>
+  </si>
+  <si>
+    <t>87.229% (+/- 1.620%)</t>
+  </si>
+  <si>
+    <t>87.741% (+/- 1.356%)</t>
+  </si>
+  <si>
+    <t>86.909% (+/- 1.338%)</t>
+  </si>
+  <si>
+    <t>87.575% (+/- 1.222%)</t>
+  </si>
+  <si>
+    <t>86.970% (+/- 1.454%)</t>
+  </si>
+  <si>
+    <t>87.232% (+/- 1.324%)</t>
+  </si>
+  <si>
+    <t>86.544% (+/- 1.738%)</t>
+  </si>
+  <si>
+    <t>87.589% (+/- 1.739%)</t>
+  </si>
+  <si>
+    <t>86.532% (+/- 1.858%)</t>
+  </si>
+  <si>
+    <t>86.960% (+/- 1.795%)</t>
+  </si>
+  <si>
+    <t>86.165% (+/- 1.438%)</t>
+  </si>
+  <si>
+    <t>87.260% (+/- 1.058%)</t>
+  </si>
+  <si>
+    <t>86.654% (+/- 1.596%)</t>
+  </si>
+  <si>
+    <t>86.852% (+/- 1.362%)</t>
+  </si>
+  <si>
+    <t>84.570% (+/- 1.299%)</t>
+  </si>
+  <si>
+    <t>85.785% (+/- 1.451%)</t>
+  </si>
+  <si>
+    <t>84.606% (+/- 1.348%)</t>
+  </si>
+  <si>
+    <t>85.034% (+/- 1.381%)</t>
+  </si>
+  <si>
+    <t>86.580% (+/- 1.578%)</t>
+  </si>
+  <si>
+    <t>87.882% (+/- 1.215%)</t>
+  </si>
+  <si>
+    <t>87.371% (+/- 1.726%)</t>
+  </si>
+  <si>
+    <t>87.582% (+/- 1.488%)</t>
+  </si>
+  <si>
+    <t>87.821% (+/- 1.235%)</t>
+  </si>
+  <si>
+    <t>88.920% (+/- 1.266%)</t>
+  </si>
+  <si>
+    <t>88.443% (+/- 1.332%)</t>
+  </si>
+  <si>
+    <t>88.633% (+/- 1.278%)</t>
+  </si>
+  <si>
+    <t>82.595% (+/- 1.341%)</t>
+  </si>
+  <si>
+    <t>84.231% (+/- 1.668%)</t>
+  </si>
+  <si>
+    <t>83.193% (+/- 1.260%)</t>
+  </si>
+  <si>
+    <t>83.610% (+/- 1.387%)</t>
+  </si>
+  <si>
+    <t>83.139% (+/- 1.293%)</t>
+  </si>
+  <si>
+    <t>84.586% (+/- 1.353%)</t>
+  </si>
+  <si>
+    <t>83.852% (+/- 1.220%)</t>
+  </si>
+  <si>
+    <t>84.130% (+/- 1.210%)</t>
+  </si>
+  <si>
+    <t>84.177% (+/- 1.256%)</t>
+  </si>
+  <si>
+    <t>86.248% (+/- 1.344%)</t>
+  </si>
+  <si>
+    <t>84.356% (+/- 1.462%)</t>
+  </si>
+  <si>
+    <t>85.117% (+/- 1.303%)</t>
+  </si>
+  <si>
+    <t>81.165% (+/- 2.037%)</t>
+  </si>
+  <si>
+    <t>82.433% (+/- 2.187%)</t>
+  </si>
+  <si>
+    <t>80.791% (+/- 2.047%)</t>
+  </si>
+  <si>
+    <t>81.450% (+/- 2.053%)</t>
+  </si>
+  <si>
+    <t>89.633% (+/- 1.329%)</t>
+  </si>
+  <si>
+    <t>90.683% (+/- 1.071%)</t>
+  </si>
+  <si>
+    <t>90.052% (+/- 1.270%)</t>
+  </si>
+  <si>
+    <t>90.322% (+/- 1.174%)</t>
+  </si>
+  <si>
+    <t>89.145% (+/- 1.079%)</t>
+  </si>
+  <si>
+    <t>90.164% (+/- 1.059%)</t>
+  </si>
+  <si>
+    <t>89.541% (+/- 1.142%)</t>
+  </si>
+  <si>
+    <t>89.811% (+/- 1.094%)</t>
+  </si>
+  <si>
+    <t>84.785% (+/- 1.003%)</t>
+  </si>
+  <si>
+    <t>86.293% (+/- 1.493%)</t>
+  </si>
+  <si>
+    <t>84.911% (+/- 0.799%)</t>
+  </si>
+  <si>
+    <t>85.507% (+/- 1.083%)</t>
+  </si>
+  <si>
+    <t>83.747% (+/- 1.047%)</t>
+  </si>
+  <si>
+    <t>85.205% (+/- 1.233%)</t>
+  </si>
+  <si>
+    <t>83.533% (+/- 0.960%)</t>
+  </si>
+  <si>
+    <t>84.233% (+/- 1.044%)</t>
+  </si>
+  <si>
+    <t>87.112% (+/- 1.415%)</t>
+  </si>
+  <si>
+    <t>88.451% (+/- 1.237%)</t>
+  </si>
+  <si>
+    <t>87.378% (+/- 1.509%)</t>
+  </si>
+  <si>
+    <t>87.842% (+/- 1.355%)</t>
+  </si>
+  <si>
+    <t>88.410% (+/- 1.312%)</t>
+  </si>
+  <si>
+    <t>89.102% (+/- 1.292%)</t>
+  </si>
+  <si>
+    <t>88.651% (+/- 1.163%)</t>
+  </si>
+  <si>
+    <t>88.843% (+/- 1.211%)</t>
+  </si>
+  <si>
+    <t>83.608% (+/- 1.600%)</t>
+  </si>
+  <si>
+    <t>84.921% (+/- 1.594%)</t>
+  </si>
+  <si>
+    <t>83.776% (+/- 1.571%)</t>
+  </si>
+  <si>
+    <t>84.260% (+/- 1.574%)</t>
+  </si>
+  <si>
+    <t>82.570% (+/- 1.210%)</t>
+  </si>
+  <si>
+    <t>83.706% (+/- 1.299%)</t>
+  </si>
+  <si>
+    <t>82.469% (+/- 1.461%)</t>
+  </si>
+  <si>
+    <t>82.932% (+/- 1.232%)</t>
   </si>
 </sst>
 </file>
@@ -4563,7 +5379,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="51">
+  <cellXfs count="50">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -4691,9 +5507,6 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -5814,9 +6627,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>3</xdr:col>
-      <xdr:colOff>15754</xdr:colOff>
+      <xdr:colOff>19564</xdr:colOff>
       <xdr:row>34</xdr:row>
-      <xdr:rowOff>129760</xdr:rowOff>
+      <xdr:rowOff>133570</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -5857,9 +6670,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>2</xdr:col>
-      <xdr:colOff>1540818</xdr:colOff>
+      <xdr:colOff>1544628</xdr:colOff>
       <xdr:row>49</xdr:row>
-      <xdr:rowOff>133650</xdr:rowOff>
+      <xdr:rowOff>129840</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -5900,9 +6713,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>12</xdr:col>
-      <xdr:colOff>19253</xdr:colOff>
+      <xdr:colOff>15443</xdr:colOff>
       <xdr:row>34</xdr:row>
-      <xdr:rowOff>133572</xdr:rowOff>
+      <xdr:rowOff>129762</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -5945,7 +6758,7 @@
       <xdr:col>11</xdr:col>
       <xdr:colOff>1522045</xdr:colOff>
       <xdr:row>49</xdr:row>
-      <xdr:rowOff>132085</xdr:rowOff>
+      <xdr:rowOff>135895</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -6034,9 +6847,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>2</xdr:col>
-      <xdr:colOff>1545687</xdr:colOff>
+      <xdr:colOff>1541877</xdr:colOff>
       <xdr:row>34</xdr:row>
-      <xdr:rowOff>135055</xdr:rowOff>
+      <xdr:rowOff>131245</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -6120,9 +6933,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>11</xdr:col>
-      <xdr:colOff>1507116</xdr:colOff>
+      <xdr:colOff>1503306</xdr:colOff>
       <xdr:row>49</xdr:row>
-      <xdr:rowOff>136717</xdr:rowOff>
+      <xdr:rowOff>132907</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -6601,7 +7414,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8E8923B1-D07A-456F-A714-3288CE84B256}">
   <dimension ref="B3:G63"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView topLeftCell="A7" workbookViewId="0">
       <selection activeCell="B11" sqref="B11"/>
     </sheetView>
   </sheetViews>
@@ -7482,8 +8295,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8AFD775D-9E0A-47CA-A1F9-F372C0ABB720}">
   <dimension ref="B3:G63"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D10" sqref="D10:G10"/>
+    <sheetView topLeftCell="A40" workbookViewId="0">
+      <selection activeCell="G57" sqref="G57"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -7500,7 +8313,7 @@
         <v>4</v>
       </c>
       <c r="C3" t="s">
-        <v>719</v>
+        <v>1493</v>
       </c>
     </row>
     <row r="5" spans="2:7" x14ac:dyDescent="0.3">
@@ -7700,69 +8513,193 @@
       <c r="F16" s="34"/>
       <c r="G16" s="34"/>
     </row>
+    <row r="18" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="B18" t="s">
+        <v>4</v>
+      </c>
+      <c r="C18" t="s">
+        <v>1494</v>
+      </c>
+    </row>
+    <row r="20" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="B20" s="34" t="s">
+        <v>23</v>
+      </c>
+      <c r="C20" s="34" t="s">
+        <v>24</v>
+      </c>
+      <c r="D20" s="34" t="s">
+        <v>5</v>
+      </c>
+      <c r="E20" s="34" t="s">
+        <v>6</v>
+      </c>
+      <c r="F20" s="34" t="s">
+        <v>26</v>
+      </c>
+      <c r="G20" s="34" t="s">
+        <v>8</v>
+      </c>
+    </row>
     <row r="21" spans="2:7" x14ac:dyDescent="0.3">
-      <c r="B21" s="34"/>
-      <c r="C21" s="34"/>
-      <c r="D21" s="34"/>
-      <c r="E21" s="34"/>
-      <c r="F21" s="34"/>
-      <c r="G21" s="34"/>
+      <c r="B21" s="4">
+        <v>12</v>
+      </c>
+      <c r="C21" s="4" t="s">
+        <v>1495</v>
+      </c>
+      <c r="D21" s="4" t="s">
+        <v>1496</v>
+      </c>
+      <c r="E21" s="4" t="s">
+        <v>1497</v>
+      </c>
+      <c r="F21" s="4" t="s">
+        <v>1498</v>
+      </c>
+      <c r="G21" s="4" t="s">
+        <v>1499</v>
+      </c>
     </row>
     <row r="22" spans="2:7" x14ac:dyDescent="0.3">
-      <c r="B22" s="4"/>
-      <c r="C22" s="4"/>
-      <c r="D22" s="4"/>
-      <c r="E22" s="4"/>
-      <c r="F22" s="4"/>
-      <c r="G22" s="4"/>
+      <c r="B22" s="34">
+        <v>11</v>
+      </c>
+      <c r="C22" s="34" t="s">
+        <v>1349</v>
+      </c>
+      <c r="D22" s="34" t="s">
+        <v>1500</v>
+      </c>
+      <c r="E22" s="34" t="s">
+        <v>1501</v>
+      </c>
+      <c r="F22" s="34" t="s">
+        <v>1528</v>
+      </c>
+      <c r="G22" s="34" t="s">
+        <v>1529</v>
+      </c>
     </row>
     <row r="23" spans="2:7" x14ac:dyDescent="0.3">
-      <c r="B23" s="34"/>
-      <c r="C23" s="34"/>
-      <c r="D23" s="34"/>
-      <c r="E23" s="34"/>
-      <c r="F23" s="34"/>
-      <c r="G23" s="34"/>
+      <c r="B23" s="4">
+        <v>10</v>
+      </c>
+      <c r="C23" s="4" t="s">
+        <v>1354</v>
+      </c>
+      <c r="D23" s="4" t="s">
+        <v>1502</v>
+      </c>
+      <c r="E23" s="4" t="s">
+        <v>1503</v>
+      </c>
+      <c r="F23" s="4" t="s">
+        <v>1504</v>
+      </c>
+      <c r="G23" s="4" t="s">
+        <v>1505</v>
+      </c>
     </row>
     <row r="24" spans="2:7" x14ac:dyDescent="0.3">
-      <c r="B24" s="4"/>
-      <c r="C24" s="13"/>
-      <c r="D24" s="4"/>
-      <c r="E24" s="4"/>
-      <c r="F24" s="4"/>
-      <c r="G24" s="4"/>
+      <c r="B24" s="34">
+        <v>9</v>
+      </c>
+      <c r="C24" s="15" t="s">
+        <v>1506</v>
+      </c>
+      <c r="D24" s="34" t="s">
+        <v>1507</v>
+      </c>
+      <c r="E24" s="34" t="s">
+        <v>1508</v>
+      </c>
+      <c r="F24" s="34" t="s">
+        <v>1509</v>
+      </c>
+      <c r="G24" s="34" t="s">
+        <v>1510</v>
+      </c>
     </row>
     <row r="25" spans="2:7" x14ac:dyDescent="0.3">
-      <c r="B25" s="34"/>
-      <c r="C25" s="15"/>
-      <c r="D25" s="34"/>
-      <c r="E25" s="34"/>
-      <c r="F25" s="34"/>
-      <c r="G25" s="34"/>
+      <c r="B25" s="4">
+        <v>8</v>
+      </c>
+      <c r="C25" s="4" t="s">
+        <v>1369</v>
+      </c>
+      <c r="D25" s="4" t="s">
+        <v>1511</v>
+      </c>
+      <c r="E25" s="4" t="s">
+        <v>1512</v>
+      </c>
+      <c r="F25" s="4" t="s">
+        <v>1513</v>
+      </c>
+      <c r="G25" s="4" t="s">
+        <v>1514</v>
+      </c>
     </row>
     <row r="26" spans="2:7" x14ac:dyDescent="0.3">
-      <c r="B26" s="3"/>
-      <c r="C26" s="3"/>
-      <c r="D26" s="3"/>
-      <c r="E26" s="3"/>
-      <c r="F26" s="3"/>
-      <c r="G26" s="3"/>
+      <c r="B26" s="4">
+        <v>7</v>
+      </c>
+      <c r="C26" s="4" t="s">
+        <v>1515</v>
+      </c>
+      <c r="D26" s="4" t="s">
+        <v>1516</v>
+      </c>
+      <c r="E26" s="4" t="s">
+        <v>1517</v>
+      </c>
+      <c r="F26" s="4" t="s">
+        <v>1518</v>
+      </c>
+      <c r="G26" s="4" t="s">
+        <v>1519</v>
+      </c>
     </row>
     <row r="27" spans="2:7" x14ac:dyDescent="0.3">
-      <c r="B27" s="4"/>
-      <c r="C27" s="4"/>
-      <c r="D27" s="4"/>
-      <c r="E27" s="4"/>
-      <c r="F27" s="4"/>
-      <c r="G27" s="4"/>
+      <c r="B27" s="3">
+        <v>6</v>
+      </c>
+      <c r="C27" s="3" t="s">
+        <v>1374</v>
+      </c>
+      <c r="D27" s="3" t="s">
+        <v>1520</v>
+      </c>
+      <c r="E27" s="3" t="s">
+        <v>1521</v>
+      </c>
+      <c r="F27" s="3" t="s">
+        <v>1522</v>
+      </c>
+      <c r="G27" s="3" t="s">
+        <v>1523</v>
+      </c>
     </row>
     <row r="28" spans="2:7" x14ac:dyDescent="0.3">
-      <c r="B28" s="34"/>
-      <c r="C28" s="13"/>
-      <c r="D28" s="34"/>
-      <c r="E28" s="34"/>
-      <c r="F28" s="34"/>
-      <c r="G28" s="34"/>
+      <c r="B28" s="34">
+        <v>5</v>
+      </c>
+      <c r="C28" s="34" t="s">
+        <v>1379</v>
+      </c>
+      <c r="D28" s="34" t="s">
+        <v>1524</v>
+      </c>
+      <c r="E28" s="34" t="s">
+        <v>1525</v>
+      </c>
+      <c r="F28" s="34" t="s">
+        <v>1526</v>
+      </c>
+      <c r="G28" s="34" t="s">
+        <v>1527</v>
+      </c>
     </row>
     <row r="29" spans="2:7" x14ac:dyDescent="0.3">
       <c r="B29" s="34"/>
@@ -7781,69 +8718,193 @@
       <c r="B32" s="36"/>
       <c r="C32" s="36"/>
     </row>
+    <row r="34" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="B34" t="s">
+        <v>4</v>
+      </c>
+      <c r="C34" t="s">
+        <v>1530</v>
+      </c>
+    </row>
+    <row r="36" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="B36" s="34" t="s">
+        <v>23</v>
+      </c>
+      <c r="C36" s="34" t="s">
+        <v>24</v>
+      </c>
+      <c r="D36" s="34" t="s">
+        <v>5</v>
+      </c>
+      <c r="E36" s="34" t="s">
+        <v>6</v>
+      </c>
+      <c r="F36" s="34" t="s">
+        <v>26</v>
+      </c>
+      <c r="G36" s="34" t="s">
+        <v>8</v>
+      </c>
+    </row>
     <row r="37" spans="2:7" x14ac:dyDescent="0.3">
-      <c r="B37" s="34"/>
-      <c r="C37" s="34"/>
-      <c r="D37" s="34"/>
-      <c r="E37" s="34"/>
-      <c r="F37" s="34"/>
-      <c r="G37" s="34"/>
+      <c r="B37" s="4">
+        <v>12</v>
+      </c>
+      <c r="C37" s="4" t="s">
+        <v>1348</v>
+      </c>
+      <c r="D37" s="4" t="s">
+        <v>1531</v>
+      </c>
+      <c r="E37" s="4" t="s">
+        <v>1532</v>
+      </c>
+      <c r="F37" s="4" t="s">
+        <v>1533</v>
+      </c>
+      <c r="G37" s="4" t="s">
+        <v>1534</v>
+      </c>
     </row>
     <row r="38" spans="2:7" x14ac:dyDescent="0.3">
-      <c r="B38" s="4"/>
-      <c r="C38" s="4"/>
-      <c r="D38" s="4"/>
-      <c r="E38" s="4"/>
-      <c r="F38" s="4"/>
-      <c r="G38" s="4"/>
+      <c r="B38" s="34">
+        <v>11</v>
+      </c>
+      <c r="C38" s="34" t="s">
+        <v>1349</v>
+      </c>
+      <c r="D38" s="34" t="s">
+        <v>1535</v>
+      </c>
+      <c r="E38" s="34" t="s">
+        <v>1536</v>
+      </c>
+      <c r="F38" s="34" t="s">
+        <v>1537</v>
+      </c>
+      <c r="G38" s="34" t="s">
+        <v>1538</v>
+      </c>
     </row>
     <row r="39" spans="2:7" x14ac:dyDescent="0.3">
-      <c r="B39" s="34"/>
-      <c r="C39" s="34"/>
-      <c r="D39" s="34"/>
-      <c r="E39" s="34"/>
-      <c r="F39" s="34"/>
-      <c r="G39" s="34"/>
+      <c r="B39" s="4">
+        <v>10</v>
+      </c>
+      <c r="C39" s="4" t="s">
+        <v>1354</v>
+      </c>
+      <c r="D39" s="4" t="s">
+        <v>1539</v>
+      </c>
+      <c r="E39" s="4" t="s">
+        <v>1540</v>
+      </c>
+      <c r="F39" s="4" t="s">
+        <v>1541</v>
+      </c>
+      <c r="G39" s="4" t="s">
+        <v>1542</v>
+      </c>
     </row>
     <row r="40" spans="2:7" x14ac:dyDescent="0.3">
-      <c r="B40" s="4"/>
-      <c r="C40" s="4"/>
-      <c r="D40" s="4"/>
-      <c r="E40" s="4"/>
-      <c r="F40" s="4"/>
-      <c r="G40" s="4"/>
+      <c r="B40" s="34">
+        <v>9</v>
+      </c>
+      <c r="C40" s="15" t="s">
+        <v>1359</v>
+      </c>
+      <c r="D40" s="34" t="s">
+        <v>1543</v>
+      </c>
+      <c r="E40" s="34" t="s">
+        <v>1544</v>
+      </c>
+      <c r="F40" s="34" t="s">
+        <v>1545</v>
+      </c>
+      <c r="G40" s="34" t="s">
+        <v>1546</v>
+      </c>
     </row>
     <row r="41" spans="2:7" x14ac:dyDescent="0.3">
-      <c r="B41" s="34"/>
-      <c r="C41" s="13"/>
-      <c r="D41" s="34"/>
-      <c r="E41" s="34"/>
-      <c r="F41" s="34"/>
-      <c r="G41" s="34"/>
+      <c r="B41" s="3">
+        <v>8</v>
+      </c>
+      <c r="C41" s="3" t="s">
+        <v>1369</v>
+      </c>
+      <c r="D41" s="3" t="s">
+        <v>1547</v>
+      </c>
+      <c r="E41" s="3" t="s">
+        <v>1548</v>
+      </c>
+      <c r="F41" s="3" t="s">
+        <v>1549</v>
+      </c>
+      <c r="G41" s="3" t="s">
+        <v>1550</v>
+      </c>
     </row>
     <row r="42" spans="2:7" x14ac:dyDescent="0.3">
-      <c r="B42" s="34"/>
-      <c r="C42" s="34"/>
-      <c r="D42" s="34"/>
-      <c r="E42" s="34"/>
-      <c r="F42" s="34"/>
-      <c r="G42" s="34"/>
+      <c r="B42" s="4">
+        <v>7</v>
+      </c>
+      <c r="C42" s="4" t="s">
+        <v>1515</v>
+      </c>
+      <c r="D42" s="4" t="s">
+        <v>1551</v>
+      </c>
+      <c r="E42" s="4" t="s">
+        <v>1552</v>
+      </c>
+      <c r="F42" s="4" t="s">
+        <v>1553</v>
+      </c>
+      <c r="G42" s="4" t="s">
+        <v>1554</v>
+      </c>
     </row>
     <row r="43" spans="2:7" x14ac:dyDescent="0.3">
-      <c r="B43" s="3"/>
-      <c r="C43" s="3"/>
-      <c r="D43" s="3"/>
-      <c r="E43" s="3"/>
-      <c r="F43" s="3"/>
-      <c r="G43" s="3"/>
+      <c r="B43" s="4">
+        <v>6</v>
+      </c>
+      <c r="C43" s="4" t="s">
+        <v>1374</v>
+      </c>
+      <c r="D43" s="4" t="s">
+        <v>1555</v>
+      </c>
+      <c r="E43" s="4" t="s">
+        <v>1556</v>
+      </c>
+      <c r="F43" s="4" t="s">
+        <v>1557</v>
+      </c>
+      <c r="G43" s="4" t="s">
+        <v>1558</v>
+      </c>
     </row>
     <row r="44" spans="2:7" x14ac:dyDescent="0.3">
-      <c r="B44" s="34"/>
-      <c r="C44" s="34"/>
-      <c r="D44" s="34"/>
-      <c r="E44" s="34"/>
-      <c r="F44" s="34"/>
-      <c r="G44" s="34"/>
+      <c r="B44" s="34">
+        <v>5</v>
+      </c>
+      <c r="C44" s="34" t="s">
+        <v>1379</v>
+      </c>
+      <c r="D44" s="34" t="s">
+        <v>1559</v>
+      </c>
+      <c r="E44" s="34" t="s">
+        <v>1560</v>
+      </c>
+      <c r="F44" s="34" t="s">
+        <v>1561</v>
+      </c>
+      <c r="G44" s="34" t="s">
+        <v>1562</v>
+      </c>
     </row>
     <row r="45" spans="2:7" x14ac:dyDescent="0.3">
       <c r="B45" s="34"/>
@@ -7866,77 +8927,193 @@
       <c r="F48" s="34"/>
       <c r="G48" s="34"/>
     </row>
+    <row r="50" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="B50" t="s">
+        <v>4</v>
+      </c>
+      <c r="C50" t="s">
+        <v>1583</v>
+      </c>
+    </row>
     <row r="52" spans="2:7" x14ac:dyDescent="0.3">
-      <c r="B52" s="34"/>
-      <c r="C52" s="34"/>
-      <c r="D52" s="34"/>
-      <c r="E52" s="34"/>
-      <c r="F52" s="34"/>
-      <c r="G52" s="34"/>
+      <c r="B52" s="34" t="s">
+        <v>23</v>
+      </c>
+      <c r="C52" s="34" t="s">
+        <v>24</v>
+      </c>
+      <c r="D52" s="34" t="s">
+        <v>5</v>
+      </c>
+      <c r="E52" s="34" t="s">
+        <v>6</v>
+      </c>
+      <c r="F52" s="34" t="s">
+        <v>26</v>
+      </c>
+      <c r="G52" s="34" t="s">
+        <v>8</v>
+      </c>
     </row>
     <row r="53" spans="2:7" x14ac:dyDescent="0.3">
-      <c r="B53" s="4"/>
-      <c r="C53" s="4"/>
-      <c r="D53" s="4"/>
-      <c r="E53" s="4"/>
-      <c r="F53" s="4"/>
-      <c r="G53" s="4"/>
+      <c r="B53" s="4">
+        <v>12</v>
+      </c>
+      <c r="C53" s="4" t="s">
+        <v>1348</v>
+      </c>
+      <c r="D53" s="4" t="s">
+        <v>1584</v>
+      </c>
+      <c r="E53" s="4" t="s">
+        <v>1585</v>
+      </c>
+      <c r="F53" s="4" t="s">
+        <v>1586</v>
+      </c>
+      <c r="G53" s="4" t="s">
+        <v>1587</v>
+      </c>
     </row>
     <row r="54" spans="2:7" x14ac:dyDescent="0.3">
-      <c r="B54" s="34"/>
-      <c r="C54" s="34"/>
-      <c r="D54" s="34"/>
-      <c r="E54" s="34"/>
-      <c r="F54" s="34"/>
-      <c r="G54" s="34"/>
+      <c r="B54" s="34">
+        <v>11</v>
+      </c>
+      <c r="C54" s="34" t="s">
+        <v>1349</v>
+      </c>
+      <c r="D54" s="34" t="s">
+        <v>1588</v>
+      </c>
+      <c r="E54" s="34" t="s">
+        <v>1589</v>
+      </c>
+      <c r="F54" s="34" t="s">
+        <v>1590</v>
+      </c>
+      <c r="G54" s="34" t="s">
+        <v>1591</v>
+      </c>
     </row>
     <row r="55" spans="2:7" x14ac:dyDescent="0.3">
-      <c r="B55" s="4"/>
-      <c r="C55" s="13"/>
-      <c r="D55" s="4"/>
-      <c r="E55" s="4"/>
-      <c r="F55" s="4"/>
-      <c r="G55" s="4"/>
+      <c r="B55" s="4">
+        <v>10</v>
+      </c>
+      <c r="C55" s="4" t="s">
+        <v>1354</v>
+      </c>
+      <c r="D55" s="4" t="s">
+        <v>1592</v>
+      </c>
+      <c r="E55" s="4" t="s">
+        <v>1593</v>
+      </c>
+      <c r="F55" s="4" t="s">
+        <v>1594</v>
+      </c>
+      <c r="G55" s="4" t="s">
+        <v>1595</v>
+      </c>
     </row>
     <row r="56" spans="2:7" x14ac:dyDescent="0.3">
-      <c r="B56" s="34"/>
-      <c r="C56" s="15"/>
-      <c r="D56" s="34"/>
-      <c r="E56" s="34"/>
-      <c r="F56" s="34"/>
-      <c r="G56" s="34"/>
+      <c r="B56" s="34">
+        <v>9</v>
+      </c>
+      <c r="C56" s="15" t="s">
+        <v>1506</v>
+      </c>
+      <c r="D56" s="34" t="s">
+        <v>1596</v>
+      </c>
+      <c r="E56" s="34" t="s">
+        <v>1597</v>
+      </c>
+      <c r="F56" s="34" t="s">
+        <v>1598</v>
+      </c>
+      <c r="G56" s="34" t="s">
+        <v>1599</v>
+      </c>
     </row>
     <row r="57" spans="2:7" x14ac:dyDescent="0.3">
-      <c r="B57" s="3"/>
-      <c r="C57" s="3"/>
-      <c r="D57" s="3"/>
-      <c r="E57" s="3"/>
-      <c r="F57" s="3"/>
-      <c r="G57" s="3"/>
+      <c r="B57" s="3">
+        <v>8</v>
+      </c>
+      <c r="C57" s="3" t="s">
+        <v>1369</v>
+      </c>
+      <c r="D57" s="4" t="s">
+        <v>1600</v>
+      </c>
+      <c r="E57" s="4" t="s">
+        <v>1601</v>
+      </c>
+      <c r="F57" s="3" t="s">
+        <v>1602</v>
+      </c>
+      <c r="G57" s="3" t="s">
+        <v>1603</v>
+      </c>
     </row>
     <row r="58" spans="2:7" x14ac:dyDescent="0.3">
-      <c r="B58" s="4"/>
-      <c r="C58" s="4"/>
-      <c r="D58" s="4"/>
-      <c r="E58" s="4"/>
-      <c r="F58" s="4"/>
-      <c r="G58" s="4"/>
+      <c r="B58" s="4">
+        <v>7</v>
+      </c>
+      <c r="C58" s="4" t="s">
+        <v>1604</v>
+      </c>
+      <c r="D58" s="4" t="s">
+        <v>1653</v>
+      </c>
+      <c r="E58" s="4" t="s">
+        <v>1654</v>
+      </c>
+      <c r="F58" s="4" t="s">
+        <v>1655</v>
+      </c>
+      <c r="G58" s="4" t="s">
+        <v>1656</v>
+      </c>
     </row>
     <row r="59" spans="2:7" x14ac:dyDescent="0.3">
-      <c r="B59" s="34"/>
-      <c r="C59" s="13"/>
-      <c r="D59" s="34"/>
-      <c r="E59" s="34"/>
-      <c r="F59" s="34"/>
-      <c r="G59" s="34"/>
+      <c r="B59" s="4">
+        <v>6</v>
+      </c>
+      <c r="C59" s="4" t="s">
+        <v>1374</v>
+      </c>
+      <c r="D59" s="4" t="s">
+        <v>1657</v>
+      </c>
+      <c r="E59" s="4" t="s">
+        <v>1658</v>
+      </c>
+      <c r="F59" s="4" t="s">
+        <v>1659</v>
+      </c>
+      <c r="G59" s="4" t="s">
+        <v>1660</v>
+      </c>
     </row>
     <row r="60" spans="2:7" x14ac:dyDescent="0.3">
-      <c r="B60" s="34"/>
-      <c r="C60" s="34"/>
-      <c r="D60" s="34"/>
-      <c r="E60" s="34"/>
-      <c r="F60" s="34"/>
-      <c r="G60" s="34"/>
+      <c r="B60" s="34">
+        <v>5</v>
+      </c>
+      <c r="C60" s="34" t="s">
+        <v>1379</v>
+      </c>
+      <c r="D60" s="34" t="s">
+        <v>1661</v>
+      </c>
+      <c r="E60" s="34" t="s">
+        <v>1662</v>
+      </c>
+      <c r="F60" s="34" t="s">
+        <v>1663</v>
+      </c>
+      <c r="G60" s="34" t="s">
+        <v>1664</v>
+      </c>
     </row>
     <row r="62" spans="2:7" x14ac:dyDescent="0.3">
       <c r="B62" s="6"/>
@@ -8786,8 +9963,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{13495555-31D4-4576-9C86-E21C2334E536}">
   <dimension ref="A2:V67"/>
   <sheetViews>
-    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="H14" sqref="H14"/>
+    <sheetView topLeftCell="B1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="G24" sqref="G24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -8916,10 +10093,18 @@
       <c r="F6" s="10" t="s">
         <v>967</v>
       </c>
-      <c r="G6" s="10"/>
-      <c r="H6" s="10"/>
-      <c r="I6" s="10"/>
-      <c r="J6" s="10"/>
+      <c r="G6" s="10" t="s">
+        <v>1469</v>
+      </c>
+      <c r="H6" s="10" t="s">
+        <v>1470</v>
+      </c>
+      <c r="I6" s="10" t="s">
+        <v>1471</v>
+      </c>
+      <c r="J6" s="10" t="s">
+        <v>1472</v>
+      </c>
       <c r="K6" s="10" t="s">
         <v>652</v>
       </c>
@@ -8960,10 +10145,18 @@
       <c r="F7" s="10" t="s">
         <v>963</v>
       </c>
-      <c r="G7" s="10"/>
-      <c r="H7" s="10"/>
-      <c r="I7" s="10"/>
-      <c r="J7" s="10"/>
+      <c r="G7" s="10" t="s">
+        <v>1473</v>
+      </c>
+      <c r="H7" s="10" t="s">
+        <v>1474</v>
+      </c>
+      <c r="I7" s="10" t="s">
+        <v>1475</v>
+      </c>
+      <c r="J7" s="10" t="s">
+        <v>1476</v>
+      </c>
       <c r="K7" s="9" t="s">
         <v>656</v>
       </c>
@@ -9006,10 +10199,18 @@
       <c r="F8" s="10" t="s">
         <v>1283</v>
       </c>
-      <c r="G8" s="10"/>
-      <c r="H8" s="10"/>
-      <c r="I8" s="10"/>
-      <c r="J8" s="10"/>
+      <c r="G8" s="10" t="s">
+        <v>1477</v>
+      </c>
+      <c r="H8" s="10" t="s">
+        <v>1478</v>
+      </c>
+      <c r="I8" s="10" t="s">
+        <v>1479</v>
+      </c>
+      <c r="J8" s="10" t="s">
+        <v>1480</v>
+      </c>
       <c r="K8" s="28" t="s">
         <v>1312</v>
       </c>
@@ -9043,10 +10244,18 @@
       <c r="F9" s="10" t="s">
         <v>1287</v>
       </c>
-      <c r="G9" s="10"/>
-      <c r="H9" s="10"/>
-      <c r="I9" s="10"/>
-      <c r="J9" s="10"/>
+      <c r="G9" s="10" t="s">
+        <v>1481</v>
+      </c>
+      <c r="H9" s="10" t="s">
+        <v>1482</v>
+      </c>
+      <c r="I9" s="10" t="s">
+        <v>1483</v>
+      </c>
+      <c r="J9" s="10" t="s">
+        <v>1484</v>
+      </c>
       <c r="K9" s="28" t="s">
         <v>1316</v>
       </c>
@@ -9082,10 +10291,18 @@
       <c r="F10" s="10" t="s">
         <v>971</v>
       </c>
-      <c r="G10" s="10"/>
-      <c r="H10" s="10"/>
-      <c r="I10" s="10"/>
-      <c r="J10" s="10"/>
+      <c r="G10" s="10" t="s">
+        <v>1485</v>
+      </c>
+      <c r="H10" s="10" t="s">
+        <v>1486</v>
+      </c>
+      <c r="I10" s="10" t="s">
+        <v>1487</v>
+      </c>
+      <c r="J10" s="10" t="s">
+        <v>1488</v>
+      </c>
       <c r="K10" s="10" t="s">
         <v>676</v>
       </c>
@@ -9126,10 +10343,18 @@
       <c r="F11" s="9" t="s">
         <v>975</v>
       </c>
-      <c r="G11" s="35"/>
-      <c r="H11" s="35"/>
-      <c r="I11" s="35"/>
-      <c r="J11" s="35"/>
+      <c r="G11" s="35" t="s">
+        <v>1489</v>
+      </c>
+      <c r="H11" s="35" t="s">
+        <v>1490</v>
+      </c>
+      <c r="I11" s="35" t="s">
+        <v>1491</v>
+      </c>
+      <c r="J11" s="35" t="s">
+        <v>1492</v>
+      </c>
       <c r="K11" s="9" t="s">
         <v>680</v>
       </c>
@@ -9172,10 +10397,18 @@
       <c r="F12" s="9" t="s">
         <v>614</v>
       </c>
-      <c r="G12" s="35"/>
-      <c r="H12" s="35"/>
-      <c r="I12" s="35"/>
-      <c r="J12" s="35"/>
+      <c r="G12" s="35" t="s">
+        <v>1461</v>
+      </c>
+      <c r="H12" s="35" t="s">
+        <v>1462</v>
+      </c>
+      <c r="I12" s="35" t="s">
+        <v>1463</v>
+      </c>
+      <c r="J12" s="35" t="s">
+        <v>1464</v>
+      </c>
       <c r="K12" s="9" t="s">
         <v>691</v>
       </c>
@@ -9216,10 +10449,18 @@
       <c r="F13" s="10" t="s">
         <v>618</v>
       </c>
-      <c r="G13" s="10"/>
-      <c r="H13" s="10"/>
-      <c r="I13" s="10"/>
-      <c r="J13" s="10"/>
+      <c r="G13" s="10" t="s">
+        <v>1465</v>
+      </c>
+      <c r="H13" s="10" t="s">
+        <v>1466</v>
+      </c>
+      <c r="I13" s="10" t="s">
+        <v>1467</v>
+      </c>
+      <c r="J13" s="10" t="s">
+        <v>1468</v>
+      </c>
       <c r="K13" s="10" t="s">
         <v>695</v>
       </c>
@@ -9262,10 +10503,18 @@
       <c r="F14" s="9" t="s">
         <v>606</v>
       </c>
-      <c r="G14" s="35"/>
-      <c r="H14" s="35"/>
-      <c r="I14" s="35"/>
-      <c r="J14" s="35"/>
+      <c r="G14" s="35" t="s">
+        <v>1453</v>
+      </c>
+      <c r="H14" s="35" t="s">
+        <v>1454</v>
+      </c>
+      <c r="I14" s="35" t="s">
+        <v>1455</v>
+      </c>
+      <c r="J14" s="35" t="s">
+        <v>1456</v>
+      </c>
       <c r="K14" s="9" t="s">
         <v>864</v>
       </c>
@@ -9306,10 +10555,18 @@
       <c r="F15" s="9" t="s">
         <v>610</v>
       </c>
-      <c r="G15" s="35"/>
-      <c r="H15" s="35"/>
-      <c r="I15" s="35"/>
-      <c r="J15" s="35"/>
+      <c r="G15" s="35" t="s">
+        <v>1457</v>
+      </c>
+      <c r="H15" s="35" t="s">
+        <v>1458</v>
+      </c>
+      <c r="I15" s="35" t="s">
+        <v>1459</v>
+      </c>
+      <c r="J15" s="35" t="s">
+        <v>1460</v>
+      </c>
       <c r="K15" s="9" t="s">
         <v>868</v>
       </c>
@@ -9404,10 +10661,18 @@
       <c r="F17" s="11" t="s">
         <v>751</v>
       </c>
-      <c r="G17" s="11"/>
-      <c r="H17" s="11"/>
-      <c r="I17" s="11"/>
-      <c r="J17" s="11"/>
+      <c r="G17" s="10" t="s">
+        <v>1449</v>
+      </c>
+      <c r="H17" s="10" t="s">
+        <v>1450</v>
+      </c>
+      <c r="I17" s="10" t="s">
+        <v>1451</v>
+      </c>
+      <c r="J17" s="10" t="s">
+        <v>1452</v>
+      </c>
       <c r="K17" s="10" t="s">
         <v>952</v>
       </c>
@@ -9602,16 +10867,16 @@
       <c r="F21" s="10" t="s">
         <v>1178</v>
       </c>
-      <c r="G21" s="10" t="s">
+      <c r="G21" s="11" t="s">
         <v>1421</v>
       </c>
-      <c r="H21" s="10" t="s">
+      <c r="H21" s="11" t="s">
         <v>1422</v>
       </c>
-      <c r="I21" s="10" t="s">
+      <c r="I21" s="11" t="s">
         <v>1423</v>
       </c>
-      <c r="J21" s="10" t="s">
+      <c r="J21" s="11" t="s">
         <v>1424</v>
       </c>
       <c r="K21" s="11" t="s">
@@ -10245,8 +11510,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B7BDEE5B-F941-4815-9630-CCD6C7441D26}">
   <dimension ref="A2:O49"/>
   <sheetViews>
-    <sheetView zoomScale="85" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="G15" sqref="G15"/>
+    <sheetView topLeftCell="B1" zoomScale="85" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="G16" sqref="G16:J16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -10355,10 +11620,18 @@
       <c r="F6" s="10" t="s">
         <v>631</v>
       </c>
-      <c r="G6" s="10"/>
-      <c r="H6" s="10"/>
-      <c r="I6" s="10"/>
-      <c r="J6" s="10"/>
+      <c r="G6" s="10" t="s">
+        <v>1621</v>
+      </c>
+      <c r="H6" s="10" t="s">
+        <v>1622</v>
+      </c>
+      <c r="I6" s="10" t="s">
+        <v>1623</v>
+      </c>
+      <c r="J6" s="10" t="s">
+        <v>1624</v>
+      </c>
       <c r="K6" s="10" t="s">
         <v>660</v>
       </c>
@@ -10389,10 +11662,18 @@
       <c r="F7" s="9" t="s">
         <v>635</v>
       </c>
-      <c r="G7" s="35"/>
-      <c r="H7" s="35"/>
-      <c r="I7" s="35"/>
-      <c r="J7" s="35"/>
+      <c r="G7" s="35" t="s">
+        <v>1625</v>
+      </c>
+      <c r="H7" s="35" t="s">
+        <v>1626</v>
+      </c>
+      <c r="I7" s="35" t="s">
+        <v>1627</v>
+      </c>
+      <c r="J7" s="35" t="s">
+        <v>1628</v>
+      </c>
       <c r="K7" s="9" t="s">
         <v>664</v>
       </c>
@@ -10425,10 +11706,18 @@
       <c r="F8" s="10" t="s">
         <v>639</v>
       </c>
-      <c r="G8" s="10"/>
-      <c r="H8" s="10"/>
-      <c r="I8" s="10"/>
-      <c r="J8" s="10"/>
+      <c r="G8" s="10" t="s">
+        <v>1605</v>
+      </c>
+      <c r="H8" s="10" t="s">
+        <v>1606</v>
+      </c>
+      <c r="I8" s="10" t="s">
+        <v>1607</v>
+      </c>
+      <c r="J8" s="10" t="s">
+        <v>1608</v>
+      </c>
       <c r="K8" s="10" t="s">
         <v>683</v>
       </c>
@@ -10459,10 +11748,18 @@
       <c r="F9" s="9" t="s">
         <v>643</v>
       </c>
-      <c r="G9" s="35"/>
-      <c r="H9" s="35"/>
-      <c r="I9" s="35"/>
-      <c r="J9" s="35"/>
+      <c r="G9" s="35" t="s">
+        <v>1609</v>
+      </c>
+      <c r="H9" s="35" t="s">
+        <v>1610</v>
+      </c>
+      <c r="I9" s="35" t="s">
+        <v>1611</v>
+      </c>
+      <c r="J9" s="35" t="s">
+        <v>1612</v>
+      </c>
       <c r="K9" s="9" t="s">
         <v>687</v>
       </c>
@@ -10495,10 +11792,18 @@
       <c r="F10" s="28" t="s">
         <v>1291</v>
       </c>
-      <c r="G10" s="35"/>
-      <c r="H10" s="35"/>
-      <c r="I10" s="35"/>
-      <c r="J10" s="35"/>
+      <c r="G10" s="35" t="s">
+        <v>1613</v>
+      </c>
+      <c r="H10" s="35" t="s">
+        <v>1614</v>
+      </c>
+      <c r="I10" s="35" t="s">
+        <v>1615</v>
+      </c>
+      <c r="J10" s="35" t="s">
+        <v>1616</v>
+      </c>
       <c r="K10" s="28" t="s">
         <v>1320</v>
       </c>
@@ -10529,10 +11834,18 @@
       <c r="F11" s="28" t="s">
         <v>1295</v>
       </c>
-      <c r="G11" s="35"/>
-      <c r="H11" s="35"/>
-      <c r="I11" s="35"/>
-      <c r="J11" s="35"/>
+      <c r="G11" s="35" t="s">
+        <v>1617</v>
+      </c>
+      <c r="H11" s="35" t="s">
+        <v>1618</v>
+      </c>
+      <c r="I11" s="35" t="s">
+        <v>1619</v>
+      </c>
+      <c r="J11" s="35" t="s">
+        <v>1620</v>
+      </c>
       <c r="K11" s="28" t="s">
         <v>1324</v>
       </c>
@@ -10565,10 +11878,18 @@
       <c r="F12" s="9" t="s">
         <v>623</v>
       </c>
-      <c r="G12" s="35"/>
-      <c r="H12" s="35"/>
-      <c r="I12" s="35"/>
-      <c r="J12" s="35"/>
+      <c r="G12" s="35" t="s">
+        <v>1579</v>
+      </c>
+      <c r="H12" s="35" t="s">
+        <v>1580</v>
+      </c>
+      <c r="I12" s="35" t="s">
+        <v>1581</v>
+      </c>
+      <c r="J12" s="35" t="s">
+        <v>1582</v>
+      </c>
       <c r="K12" s="9" t="s">
         <v>699</v>
       </c>
@@ -10599,10 +11920,18 @@
       <c r="F13" s="10" t="s">
         <v>627</v>
       </c>
-      <c r="G13" s="10"/>
-      <c r="H13" s="10"/>
-      <c r="I13" s="10"/>
-      <c r="J13" s="10"/>
+      <c r="G13" s="10" t="s">
+        <v>1465</v>
+      </c>
+      <c r="H13" s="10" t="s">
+        <v>1466</v>
+      </c>
+      <c r="I13" s="10" t="s">
+        <v>1467</v>
+      </c>
+      <c r="J13" s="10" t="s">
+        <v>1468</v>
+      </c>
       <c r="K13" s="9" t="s">
         <v>703</v>
       </c>
@@ -10635,10 +11964,18 @@
       <c r="F14" s="9" t="s">
         <v>647</v>
       </c>
-      <c r="G14" s="35"/>
-      <c r="H14" s="35"/>
-      <c r="I14" s="35"/>
-      <c r="J14" s="35"/>
+      <c r="G14" s="35" t="s">
+        <v>1571</v>
+      </c>
+      <c r="H14" s="35" t="s">
+        <v>1572</v>
+      </c>
+      <c r="I14" s="35" t="s">
+        <v>1573</v>
+      </c>
+      <c r="J14" s="35" t="s">
+        <v>1574</v>
+      </c>
       <c r="K14" s="29" t="s">
         <v>1267</v>
       </c>
@@ -10669,10 +12006,18 @@
       <c r="F15" s="9" t="s">
         <v>651</v>
       </c>
-      <c r="G15" s="35"/>
-      <c r="H15" s="35"/>
-      <c r="I15" s="35"/>
-      <c r="J15" s="35"/>
+      <c r="G15" s="35" t="s">
+        <v>1575</v>
+      </c>
+      <c r="H15" s="35" t="s">
+        <v>1576</v>
+      </c>
+      <c r="I15" s="35" t="s">
+        <v>1577</v>
+      </c>
+      <c r="J15" s="35" t="s">
+        <v>1578</v>
+      </c>
       <c r="K15" s="29" t="s">
         <v>1263</v>
       </c>
@@ -10705,10 +12050,18 @@
       <c r="F16" s="11" t="s">
         <v>509</v>
       </c>
-      <c r="G16" s="50"/>
-      <c r="H16" s="50"/>
-      <c r="I16" s="50"/>
-      <c r="J16" s="50"/>
+      <c r="G16" s="10" t="s">
+        <v>1520</v>
+      </c>
+      <c r="H16" s="10" t="s">
+        <v>1521</v>
+      </c>
+      <c r="I16" s="10" t="s">
+        <v>1522</v>
+      </c>
+      <c r="J16" s="10" t="s">
+        <v>1523</v>
+      </c>
       <c r="K16" s="4" t="s">
         <v>916</v>
       </c>
@@ -10739,10 +12092,18 @@
       <c r="F17" s="11" t="s">
         <v>755</v>
       </c>
-      <c r="G17" s="11"/>
-      <c r="H17" s="11"/>
-      <c r="I17" s="11"/>
-      <c r="J17" s="11"/>
+      <c r="G17" s="10" t="s">
+        <v>1563</v>
+      </c>
+      <c r="H17" s="10" t="s">
+        <v>1564</v>
+      </c>
+      <c r="I17" s="10" t="s">
+        <v>1565</v>
+      </c>
+      <c r="J17" s="10" t="s">
+        <v>1566</v>
+      </c>
       <c r="K17" s="10" t="s">
         <v>996</v>
       </c>
@@ -10861,16 +12222,16 @@
       <c r="F20" s="10" t="s">
         <v>1186</v>
       </c>
-      <c r="G20" s="10" t="s">
+      <c r="G20" s="11" t="s">
         <v>1425</v>
       </c>
-      <c r="H20" s="10" t="s">
+      <c r="H20" s="11" t="s">
         <v>1426</v>
       </c>
-      <c r="I20" s="10" t="s">
+      <c r="I20" s="11" t="s">
         <v>1427</v>
       </c>
-      <c r="J20" s="10" t="s">
+      <c r="J20" s="11" t="s">
         <v>1428</v>
       </c>
       <c r="K20" s="11" t="s">
@@ -10903,16 +12264,16 @@
       <c r="F21" s="10" t="s">
         <v>1190</v>
       </c>
-      <c r="G21" s="10" t="s">
+      <c r="G21" s="11" t="s">
         <v>1429</v>
       </c>
-      <c r="H21" s="10" t="s">
+      <c r="H21" s="11" t="s">
         <v>1430</v>
       </c>
-      <c r="I21" s="10" t="s">
+      <c r="I21" s="11" t="s">
         <v>1431</v>
       </c>
-      <c r="J21" s="10" t="s">
+      <c r="J21" s="11" t="s">
         <v>1432</v>
       </c>
       <c r="K21" s="10" t="s">
@@ -11132,7 +12493,7 @@
   <dimension ref="A2:O49"/>
   <sheetViews>
     <sheetView zoomScale="82" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="J21" sqref="J21"/>
+      <selection activeCell="J15" sqref="J15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -11241,10 +12602,18 @@
       <c r="F6" s="10" t="s">
         <v>801</v>
       </c>
-      <c r="G6" s="10"/>
-      <c r="H6" s="10"/>
-      <c r="I6" s="10"/>
-      <c r="J6" s="10"/>
+      <c r="G6" s="10" t="s">
+        <v>1629</v>
+      </c>
+      <c r="H6" s="10" t="s">
+        <v>1630</v>
+      </c>
+      <c r="I6" s="10" t="s">
+        <v>1631</v>
+      </c>
+      <c r="J6" s="10" t="s">
+        <v>1632</v>
+      </c>
       <c r="K6" s="10" t="s">
         <v>668</v>
       </c>
@@ -11275,10 +12644,18 @@
       <c r="F7" s="9" t="s">
         <v>805</v>
       </c>
-      <c r="G7" s="35"/>
-      <c r="H7" s="35"/>
-      <c r="I7" s="35"/>
-      <c r="J7" s="35"/>
+      <c r="G7" s="35" t="s">
+        <v>1633</v>
+      </c>
+      <c r="H7" s="35" t="s">
+        <v>1634</v>
+      </c>
+      <c r="I7" s="35" t="s">
+        <v>1635</v>
+      </c>
+      <c r="J7" s="35" t="s">
+        <v>1636</v>
+      </c>
       <c r="K7" s="9" t="s">
         <v>672</v>
       </c>
@@ -11311,10 +12688,18 @@
       <c r="F8" s="10" t="s">
         <v>825</v>
       </c>
-      <c r="G8" s="10"/>
-      <c r="H8" s="10"/>
-      <c r="I8" s="10"/>
-      <c r="J8" s="10"/>
+      <c r="G8" s="10" t="s">
+        <v>1645</v>
+      </c>
+      <c r="H8" s="10" t="s">
+        <v>1646</v>
+      </c>
+      <c r="I8" s="10" t="s">
+        <v>1647</v>
+      </c>
+      <c r="J8" s="10" t="s">
+        <v>1648</v>
+      </c>
       <c r="K8" s="10" t="s">
         <v>1271</v>
       </c>
@@ -11345,10 +12730,18 @@
       <c r="F9" s="9" t="s">
         <v>829</v>
       </c>
-      <c r="G9" s="35"/>
-      <c r="H9" s="35"/>
-      <c r="I9" s="35"/>
-      <c r="J9" s="35"/>
+      <c r="G9" s="35" t="s">
+        <v>1649</v>
+      </c>
+      <c r="H9" s="35" t="s">
+        <v>1650</v>
+      </c>
+      <c r="I9" s="35" t="s">
+        <v>1651</v>
+      </c>
+      <c r="J9" s="35" t="s">
+        <v>1652</v>
+      </c>
       <c r="K9" s="24" t="s">
         <v>1275</v>
       </c>
@@ -11381,10 +12774,18 @@
       <c r="F10" s="28" t="s">
         <v>1299</v>
       </c>
-      <c r="G10" s="35"/>
-      <c r="H10" s="35"/>
-      <c r="I10" s="35"/>
-      <c r="J10" s="35"/>
+      <c r="G10" s="35" t="s">
+        <v>1665</v>
+      </c>
+      <c r="H10" s="35" t="s">
+        <v>1666</v>
+      </c>
+      <c r="I10" s="35" t="s">
+        <v>1667</v>
+      </c>
+      <c r="J10" s="35" t="s">
+        <v>1668</v>
+      </c>
       <c r="K10" s="28" t="s">
         <v>1328</v>
       </c>
@@ -11415,10 +12816,18 @@
       <c r="F11" s="28" t="s">
         <v>1303</v>
       </c>
-      <c r="G11" s="35"/>
-      <c r="H11" s="35"/>
-      <c r="I11" s="35"/>
-      <c r="J11" s="35"/>
+      <c r="G11" s="35" t="s">
+        <v>1669</v>
+      </c>
+      <c r="H11" s="35" t="s">
+        <v>1670</v>
+      </c>
+      <c r="I11" s="35" t="s">
+        <v>1671</v>
+      </c>
+      <c r="J11" s="35" t="s">
+        <v>1672</v>
+      </c>
       <c r="K11" s="28" t="s">
         <v>1332</v>
       </c>
@@ -11451,10 +12860,18 @@
       <c r="F12" s="9" t="s">
         <v>841</v>
       </c>
-      <c r="G12" s="35"/>
-      <c r="H12" s="35"/>
-      <c r="I12" s="35"/>
-      <c r="J12" s="35"/>
+      <c r="G12" s="35" t="s">
+        <v>1689</v>
+      </c>
+      <c r="H12" s="35" t="s">
+        <v>1690</v>
+      </c>
+      <c r="I12" s="35" t="s">
+        <v>1691</v>
+      </c>
+      <c r="J12" s="35" t="s">
+        <v>1692</v>
+      </c>
       <c r="K12" s="9" t="s">
         <v>707</v>
       </c>
@@ -11485,10 +12902,18 @@
       <c r="F13" s="10" t="s">
         <v>845</v>
       </c>
-      <c r="G13" s="10"/>
-      <c r="H13" s="10"/>
-      <c r="I13" s="10"/>
-      <c r="J13" s="10"/>
+      <c r="G13" s="10" t="s">
+        <v>1693</v>
+      </c>
+      <c r="H13" s="10" t="s">
+        <v>1694</v>
+      </c>
+      <c r="I13" s="10" t="s">
+        <v>1695</v>
+      </c>
+      <c r="J13" s="10" t="s">
+        <v>1696</v>
+      </c>
       <c r="K13" s="10" t="s">
         <v>762</v>
       </c>
@@ -11521,10 +12946,18 @@
       <c r="F14" s="29" t="s">
         <v>777</v>
       </c>
-      <c r="G14" s="29"/>
-      <c r="H14" s="29"/>
-      <c r="I14" s="29"/>
-      <c r="J14" s="29"/>
+      <c r="G14" s="29" t="s">
+        <v>1705</v>
+      </c>
+      <c r="H14" s="29" t="s">
+        <v>1706</v>
+      </c>
+      <c r="I14" s="29" t="s">
+        <v>1707</v>
+      </c>
+      <c r="J14" s="29" t="s">
+        <v>1708</v>
+      </c>
       <c r="K14" s="29" t="s">
         <v>711</v>
       </c>
@@ -11555,10 +12988,18 @@
       <c r="F15" s="29" t="s">
         <v>781</v>
       </c>
-      <c r="G15" s="29"/>
-      <c r="H15" s="29"/>
-      <c r="I15" s="29"/>
-      <c r="J15" s="29"/>
+      <c r="G15" s="29" t="s">
+        <v>1709</v>
+      </c>
+      <c r="H15" s="29" t="s">
+        <v>1710</v>
+      </c>
+      <c r="I15" s="29" t="s">
+        <v>1711</v>
+      </c>
+      <c r="J15" s="29" t="s">
+        <v>1712</v>
+      </c>
       <c r="K15" s="29" t="s">
         <v>715</v>
       </c>
@@ -11591,10 +13032,18 @@
       <c r="F16" s="33" t="s">
         <v>546</v>
       </c>
-      <c r="G16" s="33"/>
-      <c r="H16" s="33"/>
-      <c r="I16" s="33"/>
-      <c r="J16" s="33"/>
+      <c r="G16" s="10" t="s">
+        <v>1547</v>
+      </c>
+      <c r="H16" s="10" t="s">
+        <v>1548</v>
+      </c>
+      <c r="I16" s="10" t="s">
+        <v>1549</v>
+      </c>
+      <c r="J16" s="10" t="s">
+        <v>1550</v>
+      </c>
       <c r="K16" s="30" t="s">
         <v>944</v>
       </c>
@@ -11625,10 +13074,18 @@
       <c r="F17" s="33" t="s">
         <v>759</v>
       </c>
-      <c r="G17" s="33"/>
-      <c r="H17" s="33"/>
-      <c r="I17" s="33"/>
-      <c r="J17" s="33"/>
+      <c r="G17" s="30" t="s">
+        <v>1567</v>
+      </c>
+      <c r="H17" s="30" t="s">
+        <v>1568</v>
+      </c>
+      <c r="I17" s="30" t="s">
+        <v>1569</v>
+      </c>
+      <c r="J17" s="30" t="s">
+        <v>1570</v>
+      </c>
       <c r="K17" s="30" t="s">
         <v>1033</v>
       </c>
@@ -11747,16 +13204,16 @@
       <c r="F20" s="30" t="s">
         <v>1194</v>
       </c>
-      <c r="G20" s="30" t="s">
+      <c r="G20" s="33" t="s">
         <v>1433</v>
       </c>
-      <c r="H20" s="30" t="s">
+      <c r="H20" s="33" t="s">
         <v>1434</v>
       </c>
-      <c r="I20" s="30" t="s">
+      <c r="I20" s="33" t="s">
         <v>1435</v>
       </c>
-      <c r="J20" s="30" t="s">
+      <c r="J20" s="33" t="s">
         <v>1436</v>
       </c>
       <c r="K20" s="33" t="s">
@@ -11789,16 +13246,16 @@
       <c r="F21" s="30" t="s">
         <v>1198</v>
       </c>
-      <c r="G21" s="30" t="s">
+      <c r="G21" s="33" t="s">
         <v>1437</v>
       </c>
-      <c r="H21" s="30" t="s">
+      <c r="H21" s="33" t="s">
         <v>1438</v>
       </c>
-      <c r="I21" s="30" t="s">
+      <c r="I21" s="33" t="s">
         <v>1439</v>
       </c>
-      <c r="J21" s="30" t="s">
+      <c r="J21" s="33" t="s">
         <v>1440</v>
       </c>
       <c r="K21" s="30" t="s">
@@ -12018,7 +13475,7 @@
   <dimension ref="A2:O49"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="J21" sqref="J21"/>
+      <selection activeCell="J16" sqref="C16:J17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -12127,10 +13584,18 @@
       <c r="F6" s="30" t="s">
         <v>809</v>
       </c>
-      <c r="G6" s="30"/>
-      <c r="H6" s="30"/>
-      <c r="I6" s="30"/>
-      <c r="J6" s="30"/>
+      <c r="G6" s="30" t="s">
+        <v>1637</v>
+      </c>
+      <c r="H6" s="30" t="s">
+        <v>1638</v>
+      </c>
+      <c r="I6" s="30" t="s">
+        <v>1639</v>
+      </c>
+      <c r="J6" s="30" t="s">
+        <v>1640</v>
+      </c>
       <c r="K6" s="30" t="s">
         <v>814</v>
       </c>
@@ -12161,10 +13626,18 @@
       <c r="F7" s="31" t="s">
         <v>813</v>
       </c>
-      <c r="G7" s="31"/>
-      <c r="H7" s="31"/>
-      <c r="I7" s="31"/>
-      <c r="J7" s="31"/>
+      <c r="G7" s="31" t="s">
+        <v>1641</v>
+      </c>
+      <c r="H7" s="31" t="s">
+        <v>1642</v>
+      </c>
+      <c r="I7" s="31" t="s">
+        <v>1643</v>
+      </c>
+      <c r="J7" s="31" t="s">
+        <v>1644</v>
+      </c>
       <c r="K7" s="31" t="s">
         <v>818</v>
       </c>
@@ -12197,10 +13670,18 @@
       <c r="F8" s="30" t="s">
         <v>833</v>
       </c>
-      <c r="G8" s="30"/>
-      <c r="H8" s="30"/>
-      <c r="I8" s="30"/>
-      <c r="J8" s="30"/>
+      <c r="G8" s="30" t="s">
+        <v>1681</v>
+      </c>
+      <c r="H8" s="30" t="s">
+        <v>1682</v>
+      </c>
+      <c r="I8" s="30" t="s">
+        <v>1683</v>
+      </c>
+      <c r="J8" s="30" t="s">
+        <v>1684</v>
+      </c>
       <c r="K8" s="30" t="s">
         <v>766</v>
       </c>
@@ -12231,10 +13712,18 @@
       <c r="F9" s="31" t="s">
         <v>837</v>
       </c>
-      <c r="G9" s="31"/>
-      <c r="H9" s="31"/>
-      <c r="I9" s="31"/>
-      <c r="J9" s="31"/>
+      <c r="G9" s="31" t="s">
+        <v>1685</v>
+      </c>
+      <c r="H9" s="31" t="s">
+        <v>1686</v>
+      </c>
+      <c r="I9" s="31" t="s">
+        <v>1687</v>
+      </c>
+      <c r="J9" s="31" t="s">
+        <v>1688</v>
+      </c>
       <c r="K9" s="31" t="s">
         <v>770</v>
       </c>
@@ -12267,10 +13756,18 @@
       <c r="F10" s="31" t="s">
         <v>1307</v>
       </c>
-      <c r="G10" s="31"/>
-      <c r="H10" s="31"/>
-      <c r="I10" s="31"/>
-      <c r="J10" s="31"/>
+      <c r="G10" s="31" t="s">
+        <v>1673</v>
+      </c>
+      <c r="H10" s="31" t="s">
+        <v>1674</v>
+      </c>
+      <c r="I10" s="31" t="s">
+        <v>1675</v>
+      </c>
+      <c r="J10" s="31" t="s">
+        <v>1676</v>
+      </c>
       <c r="K10" s="31" t="s">
         <v>1336</v>
       </c>
@@ -12301,10 +13798,18 @@
       <c r="F11" s="31" t="s">
         <v>1311</v>
       </c>
-      <c r="G11" s="31"/>
-      <c r="H11" s="31"/>
-      <c r="I11" s="31"/>
-      <c r="J11" s="31"/>
+      <c r="G11" s="31" t="s">
+        <v>1677</v>
+      </c>
+      <c r="H11" s="31" t="s">
+        <v>1678</v>
+      </c>
+      <c r="I11" s="31" t="s">
+        <v>1679</v>
+      </c>
+      <c r="J11" s="31" t="s">
+        <v>1680</v>
+      </c>
       <c r="K11" s="31" t="s">
         <v>1340</v>
       </c>
@@ -12337,10 +13842,18 @@
       <c r="F12" s="9" t="s">
         <v>849</v>
       </c>
-      <c r="G12" s="35"/>
-      <c r="H12" s="35"/>
-      <c r="I12" s="35"/>
-      <c r="J12" s="35"/>
+      <c r="G12" s="35" t="s">
+        <v>1697</v>
+      </c>
+      <c r="H12" s="35" t="s">
+        <v>1698</v>
+      </c>
+      <c r="I12" s="35" t="s">
+        <v>1699</v>
+      </c>
+      <c r="J12" s="35" t="s">
+        <v>1700</v>
+      </c>
       <c r="K12" s="9" t="s">
         <v>854</v>
       </c>
@@ -12371,10 +13884,18 @@
       <c r="F13" s="10" t="s">
         <v>853</v>
       </c>
-      <c r="G13" s="10"/>
-      <c r="H13" s="10"/>
-      <c r="I13" s="10"/>
-      <c r="J13" s="10"/>
+      <c r="G13" s="10" t="s">
+        <v>1701</v>
+      </c>
+      <c r="H13" s="10" t="s">
+        <v>1702</v>
+      </c>
+      <c r="I13" s="10" t="s">
+        <v>1703</v>
+      </c>
+      <c r="J13" s="10" t="s">
+        <v>1704</v>
+      </c>
       <c r="K13" s="10" t="s">
         <v>760</v>
       </c>
@@ -12407,10 +13928,18 @@
       <c r="F14" s="9" t="s">
         <v>785</v>
       </c>
-      <c r="G14" s="35"/>
-      <c r="H14" s="35"/>
-      <c r="I14" s="35"/>
-      <c r="J14" s="35"/>
+      <c r="G14" s="35" t="s">
+        <v>1713</v>
+      </c>
+      <c r="H14" s="35" t="s">
+        <v>1714</v>
+      </c>
+      <c r="I14" s="35" t="s">
+        <v>1715</v>
+      </c>
+      <c r="J14" s="35" t="s">
+        <v>1716</v>
+      </c>
       <c r="K14" s="9" t="s">
         <v>790</v>
       </c>
@@ -12441,10 +13970,18 @@
       <c r="F15" s="9" t="s">
         <v>789</v>
       </c>
-      <c r="G15" s="35"/>
-      <c r="H15" s="35"/>
-      <c r="I15" s="35"/>
-      <c r="J15" s="35"/>
+      <c r="G15" s="35" t="s">
+        <v>1717</v>
+      </c>
+      <c r="H15" s="35" t="s">
+        <v>1718</v>
+      </c>
+      <c r="I15" s="35" t="s">
+        <v>1719</v>
+      </c>
+      <c r="J15" s="35" t="s">
+        <v>1720</v>
+      </c>
       <c r="K15" s="9" t="s">
         <v>794</v>
       </c>
@@ -12477,10 +14014,18 @@
       <c r="F16" s="11" t="s">
         <v>577</v>
       </c>
-      <c r="G16" s="11"/>
-      <c r="H16" s="11"/>
-      <c r="I16" s="11"/>
-      <c r="J16" s="11"/>
+      <c r="G16" s="10" t="s">
+        <v>1600</v>
+      </c>
+      <c r="H16" s="10" t="s">
+        <v>1601</v>
+      </c>
+      <c r="I16" s="10" t="s">
+        <v>1602</v>
+      </c>
+      <c r="J16" s="10" t="s">
+        <v>1603</v>
+      </c>
       <c r="K16" s="10" t="s">
         <v>1054</v>
       </c>
@@ -12511,10 +14056,18 @@
       <c r="F17" s="11" t="s">
         <v>875</v>
       </c>
-      <c r="G17" s="11"/>
-      <c r="H17" s="11"/>
-      <c r="I17" s="11"/>
-      <c r="J17" s="11"/>
+      <c r="G17" s="10" t="s">
+        <v>1661</v>
+      </c>
+      <c r="H17" s="10" t="s">
+        <v>1662</v>
+      </c>
+      <c r="I17" s="10" t="s">
+        <v>1663</v>
+      </c>
+      <c r="J17" s="10" t="s">
+        <v>1664</v>
+      </c>
       <c r="K17" s="10" t="s">
         <v>1079</v>
       </c>
@@ -12589,16 +14142,16 @@
       <c r="F19" s="10" t="s">
         <v>1115</v>
       </c>
-      <c r="G19" s="10" t="s">
+      <c r="G19" s="11" t="s">
         <v>1413</v>
       </c>
-      <c r="H19" s="10" t="s">
+      <c r="H19" s="11" t="s">
         <v>1414</v>
       </c>
-      <c r="I19" s="10" t="s">
+      <c r="I19" s="11" t="s">
         <v>1415</v>
       </c>
-      <c r="J19" s="10" t="s">
+      <c r="J19" s="11" t="s">
         <v>1416</v>
       </c>
       <c r="K19" s="11" t="s">
@@ -12633,16 +14186,16 @@
       <c r="F20" s="10" t="s">
         <v>1206</v>
       </c>
-      <c r="G20" s="10" t="s">
+      <c r="G20" s="11" t="s">
         <v>1441</v>
       </c>
-      <c r="H20" s="10" t="s">
+      <c r="H20" s="11" t="s">
         <v>1442</v>
       </c>
-      <c r="I20" s="10" t="s">
+      <c r="I20" s="11" t="s">
         <v>1443</v>
       </c>
-      <c r="J20" s="10" t="s">
+      <c r="J20" s="11" t="s">
         <v>1444</v>
       </c>
       <c r="K20" s="11" t="s">

</xml_diff>